<commit_message>
DataPack Populator Added, Queue connections made to orchestrator (Large commit -182)
</commit_message>
<xml_diff>
--- a/Excel Templates/Admin Order Schedule Allocation.xlsx
+++ b/Excel Templates/Admin Order Schedule Allocation.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -13,15 +13,53 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>Schedule Name</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Allocated Amount</t>
+  </si>
+  <si>
+    <t>Available Amount</t>
+  </si>
+  <si>
+    <t>Payment ID</t>
+  </si>
+  <si>
+    <t>Full Path</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -32,7 +70,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -40,18 +78,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -98,7 +160,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -133,7 +195,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,13 +403,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="20.28515625" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="28.5703125" customWidth="1"/>
+    <col min="5" max="5" width="34.140625" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
+    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="11" max="11" width="14" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" customWidth="1"/>
+    <col min="13" max="13" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K14" s="2"/>
+      <c r="L14" s="2"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refunds + Allocations added, Structure changed to work without Queues
</commit_message>
<xml_diff>
--- a/Excel Templates/Admin Order Schedule Allocation.xlsx
+++ b/Excel Templates/Admin Order Schedule Allocation.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Schedule Name</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Full Path</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -407,7 +410,7 @@
   <dimension ref="A1:P14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,6 +451,9 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K14" s="2"/>

</xml_diff>